<commit_message>
Se separaron las funciones de cambiar contraseña, cambiar puntos fuertes por forms separados. Ademas de botones para navegar por el menu.
Se agrego la funcion de cambiar el horario de la clase y su hora del entrenador.
</commit_message>
<xml_diff>
--- a/Proyecto1/bin/Debug/Administrador.xlsx
+++ b/Proyecto1/bin/Debug/Administrador.xlsx
@@ -5,15 +5,15 @@
   <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\source\repos\AngeloWong09\GimnacioProyecto\Proyecto1\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69323B16-BB99-4B71-BE86-5E42E1EB39A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E910B9B5-C2B9-414F-92E2-ECF65B08B9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="11412" yWindow="2268" windowWidth="9036" windowHeight="8964" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <x:sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="124519"/>
@@ -59,7 +59,7 @@
     <x:t>Calvo</x:t>
   </x:si>
   <x:si>
-    <x:t>Patito00</x:t>
+    <x:t>0</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -492,14 +492,14 @@
   <x:dimension ref="A1:H101"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="C7" sqref="C7"/>
+      <x:selection activeCell="E6" sqref="E6"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr baseColWidth="10" defaultColWidth="8.853482" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <x:cols>
     <x:col min="1" max="1" width="12.21875" style="0" bestFit="1" customWidth="1"/>
     <x:col min="2" max="2" width="10.554688" style="0" bestFit="1" customWidth="1"/>
-    <x:col min="3" max="3" width="8.853482" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="8.886719" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="10.554688" style="0" bestFit="1" customWidth="1"/>
     <x:col min="5" max="5" width="11.441406" style="0" bestFit="1" customWidth="1"/>
     <x:col min="6" max="7" width="16.332031" style="0" bestFit="1" customWidth="1"/>

</xml_diff>